<commit_message>
Add inventory column to spreadsheet and use values to calculate stock
</commit_message>
<xml_diff>
--- a/inventory_test_data.xlsx
+++ b/inventory_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Chin\OneDrive\Documents\ENG100D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edbert\git\the-hub-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443E610F-3056-466E-B46C-F76480C94CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E39D7C-92D2-4DFF-97C7-8062548703A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9372" yWindow="3984" windowWidth="10344" windowHeight="7704" activeTab="1" xr2:uid="{74F179E7-723B-411B-9727-4BDBEF0EA843}"/>
+    <workbookView xWindow="5565" yWindow="3180" windowWidth="28800" windowHeight="15345" xr2:uid="{74F179E7-723B-411B-9727-4BDBEF0EA843}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory_test" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Item_Name</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Dryer Sheets</t>
+  </si>
+  <si>
+    <t>Inventory</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -279,12 +285,13 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{40A7002A-83E0-4E5D-803C-48C83E298371}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="7" unboundColumnsRight="1">
+    <queryTableFields count="5">
       <queryTableField id="1" name="Item_Name" tableColumnId="1"/>
       <queryTableField id="2" name="#_Of_Requests" tableColumnId="2"/>
       <queryTableField id="3" name="Extras_Requested" tableColumnId="3"/>
       <queryTableField id="4" name="Total" tableColumnId="4"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="5"/>
     </queryTableFields>
     <queryTableDeletedFields count="1">
       <deletedField name="Column1"/>
@@ -294,13 +301,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAA732C2-86E2-4886-B279-35572144EA1B}" name="inventory_test" displayName="inventory_test" ref="A1:D44" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D44" xr:uid="{DAA732C2-86E2-4886-B279-35572144EA1B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{766DA3BD-75AA-4456-BC5C-C91B3409BDDE}" uniqueName="1" name="Item_Name" queryTableFieldId="1" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DAA732C2-86E2-4886-B279-35572144EA1B}" name="inventory_test" displayName="inventory_test" ref="A1:E44" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E44" xr:uid="{DAA732C2-86E2-4886-B279-35572144EA1B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{766DA3BD-75AA-4456-BC5C-C91B3409BDDE}" uniqueName="1" name="Item_Name" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{79F0796C-044E-4E96-B8DC-AF1DFEE0B1D0}" uniqueName="2" name="#_Of_Requests" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{6D03B8BB-614C-4228-BADC-211736C29290}" uniqueName="3" name="Extras_Requested" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{E38E7A1C-C33A-474F-B701-DF33EE348AB1}" uniqueName="4" name="Total" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{FB19C23E-0144-4AF5-B647-1881459280B0}" uniqueName="5" name="Inventory" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,21 +611,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6031E1E9-F788-4BA1-8600-FD24A9A69169}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,8 +639,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -644,8 +656,11 @@
       <c r="D2">
         <v>252</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -658,8 +673,11 @@
       <c r="D3">
         <v>212</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -672,8 +690,11 @@
       <c r="D4">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -686,8 +707,11 @@
       <c r="D5">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -700,8 +724,11 @@
       <c r="D6">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -714,8 +741,11 @@
       <c r="D7">
         <v>220</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -728,8 +758,11 @@
       <c r="D8">
         <v>246</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -742,8 +775,11 @@
       <c r="D9">
         <v>243</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -756,8 +792,11 @@
       <c r="D10">
         <v>207</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -770,8 +809,11 @@
       <c r="D11">
         <v>276</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -784,8 +826,11 @@
       <c r="D12">
         <v>283</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -798,8 +843,11 @@
       <c r="D13">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -812,8 +860,11 @@
       <c r="D14">
         <v>266</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -826,8 +877,11 @@
       <c r="D15">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -840,8 +894,11 @@
       <c r="D16">
         <v>189</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -854,8 +911,11 @@
       <c r="D17">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -868,8 +928,11 @@
       <c r="D18">
         <v>189</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -882,8 +945,11 @@
       <c r="D19">
         <v>408</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -896,8 +962,11 @@
       <c r="D20">
         <v>291</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -910,8 +979,11 @@
       <c r="D21">
         <v>332</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -924,8 +996,11 @@
       <c r="D22">
         <v>245</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -938,8 +1013,11 @@
       <c r="D23">
         <v>234</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -952,8 +1030,11 @@
       <c r="D24">
         <v>203</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -966,8 +1047,11 @@
       <c r="D25">
         <v>366</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -980,8 +1064,11 @@
       <c r="D26">
         <v>252</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -994,8 +1081,11 @@
       <c r="D27">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1008,8 +1098,11 @@
       <c r="D28">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1022,8 +1115,11 @@
       <c r="D29">
         <v>145</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1036,8 +1132,11 @@
       <c r="D30">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1050,8 +1149,11 @@
       <c r="D31">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1064,8 +1166,11 @@
       <c r="D32">
         <v>199</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1078,8 +1183,11 @@
       <c r="D33">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1092,8 +1200,11 @@
       <c r="D34">
         <v>101</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1106,8 +1217,11 @@
       <c r="D35">
         <v>119</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1120,8 +1234,11 @@
       <c r="D36">
         <v>195</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1134,8 +1251,11 @@
       <c r="D37">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1148,8 +1268,11 @@
       <c r="D38">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1162,8 +1285,11 @@
       <c r="D39">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1176,8 +1302,11 @@
       <c r="D40">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1190,8 +1319,11 @@
       <c r="D41">
         <v>432</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1204,8 +1336,11 @@
       <c r="D42">
         <v>415</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1218,8 +1353,11 @@
       <c r="D43">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1231,6 +1369,9 @@
       </c>
       <c r="D44">
         <v>245</v>
+      </c>
+      <c r="E44">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1245,16 +1386,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FCD7FC-2C36-4BB7-ADC0-DA260E37AAF6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
@@ -1262,7 +1403,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1270,7 +1411,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1278,7 +1419,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1286,7 +1427,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1294,7 +1435,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>

</xml_diff>